<commit_message>
omp constant time fix + excel changes
</commit_message>
<xml_diff>
--- a/results/new_pi_matrix.xlsx
+++ b/results/new_pi_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Education\risc_v\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF49768-8A15-4DBF-9570-5CAF7AC57981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97098F94-CBC7-4293-B203-F265AED1C4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1C5123AA-3652-4661-A586-32097E39DAF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C5123AA-3652-4661-A586-32097E39DAF3}"/>
   </bookViews>
   <sheets>
     <sheet name="pi" sheetId="1" r:id="rId1"/>
@@ -747,28 +747,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.1896929218592884</c:v>
+                  <c:v>2676000.4147557071</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2741041141960912</c:v>
+                  <c:v>347546.23771274334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2856000728541135</c:v>
+                  <c:v>35158.06500137777</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3284384437496595</c:v>
+                  <c:v>3558.3963949843683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6139396627922853</c:v>
+                  <c:v>378.0332516510054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.5568705928092239</c:v>
+                  <c:v>86.177973416781896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.085090333028173</c:v>
+                  <c:v>49.193214237918355</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.970655371889009</c:v>
+                  <c:v>43.728271545286468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -846,28 +846,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0001656810075503</c:v>
+                  <c:v>2698.3985165205663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0135247779617154</c:v>
+                  <c:v>228.45607046678631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2111724837112559</c:v>
+                  <c:v>18.555620748455233</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.263431842224879</c:v>
+                  <c:v>13.216984363010521</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.334490163627169</c:v>
+                  <c:v>13.402857762988152</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.455451393022141</c:v>
+                  <c:v>14.290066016963969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.753209035579349</c:v>
+                  <c:v>26.814777216169546</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.800126031748288</c:v>
+                  <c:v>26.680664300141995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3417,28 +3417,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>27.584335385296985</c:v>
+                  <c:v>6.3803639396727159E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.167655856384414</c:v>
+                  <c:v>5.8070898215102521E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.752267284014025</c:v>
+                  <c:v>6.7493945978399951E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.502325128112012</c:v>
+                  <c:v>5.780383662200124E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31.077653870956667</c:v>
+                  <c:v>0.54372393609810599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.104527141961846</c:v>
+                  <c:v>3.8929834366719591</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.92835744506865</c:v>
+                  <c:v>7.1024857820926464</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.7260153582315869</c:v>
+                  <c:v>7.97617971916572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3693,13 +3693,6 @@
               <a:rPr lang="en-US" baseline="0"/>
               <a:t> Matebook D15 (double)</a:t>
             </a:r>
-            <a:br>
-              <a:rPr lang="ru-RU" baseline="0"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t>логарифмическая шкала</a:t>
-            </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:rich>
@@ -4003,28 +3996,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.12688935164410001</c:v>
+                  <c:v>2.9349999999999997E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1251899048748</c:v>
+                  <c:v>2.26E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1250411311563</c:v>
+                  <c:v>2.2354999999999999E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1252233435141</c:v>
+                  <c:v>2.2270375E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12722766850010001</c:v>
+                  <c:v>2.2259315000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14086739300000001</c:v>
+                  <c:v>1.5621757999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25487476662500003</c:v>
+                  <c:v>0.12996826175000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4227878419375</c:v>
+                  <c:v>1.3005261925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4102,28 +4095,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.0002655250000001E-2</c:v>
+                  <c:v>3.7075000000000001E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0044157500000001E-3</c:v>
+                  <c:v>4.4560000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.144195E-4</c:v>
+                  <c:v>1.363475E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2430349999999999E-4</c:v>
+                  <c:v>1.153355E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.131108E-3</c:v>
+                  <c:v>1.1253382499999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.12947415E-2</c:v>
+                  <c:v>1.06350695E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6541675999999999E-2</c:v>
+                  <c:v>5.6411853249999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56208813224999998</c:v>
+                  <c:v>0.56460486200000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4388,17 +4381,6 @@
                 <a:effectLst/>
               </a:rPr>
               <a:t>(double) </a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-            </a:br>
-            <a:r>
-              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>логарифмическая шкала</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -5112,7 +5094,7 @@
               <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>линейная шкала</a:t>
+              <a:t>логарифмическая шкала</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU" sz="1100">
               <a:effectLst/>
@@ -5532,6 +5514,7 @@
       <c:valAx>
         <c:axId val="1936509872"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5728,7 +5711,7 @@
               <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>линейная шкала</a:t>
+              <a:t>логарифмическая шкала</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU" sz="1100">
               <a:effectLst/>
@@ -6134,6 +6117,7 @@
       <c:valAx>
         <c:axId val="133287776"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -15108,15 +15092,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>899160</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:colOff>891540</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15145,14 +15129,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>944880</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1059180</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15772,8 +15756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E820A18-221D-4656-A150-551390AF7477}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView topLeftCell="G25" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16112,14 +16096,14 @@
         <v>8.3333333000000004E-6</v>
       </c>
       <c r="V4" s="4">
-        <v>0.12688935164410001</v>
+        <v>2.9349999999999997E-7</v>
       </c>
       <c r="W4" s="4">
         <v>4.8100000000000003E-7</v>
       </c>
       <c r="X4" s="4">
         <f>W4/V4</f>
-        <v>3.7907042140865505E-6</v>
+        <v>1.6388415672913119</v>
       </c>
       <c r="Y4" s="4">
         <v>8.3333333000000004E-6</v>
@@ -16139,11 +16123,11 @@
       </c>
       <c r="AD4" s="4">
         <f>AA4/V4</f>
-        <v>6.1896929218592884</v>
+        <v>2676000.4147557071</v>
       </c>
       <c r="AE4" s="4">
         <f>AC4/X4</f>
-        <v>27.584335385296985</v>
+        <v>6.3803639396727159E-5</v>
       </c>
       <c r="AF4" s="13">
         <v>8.3333333000000004E-6</v>
@@ -16152,14 +16136,14 @@
         <v>8.3333333000000004E-6</v>
       </c>
       <c r="AH4" s="4">
-        <v>1.0002655250000001E-2</v>
+        <v>3.7075000000000001E-6</v>
       </c>
       <c r="AI4" s="4">
         <v>1.0004312499999999E-2</v>
       </c>
       <c r="AJ4" s="4">
         <f t="shared" ref="AJ4:AJ11" si="3">AI4/AH4</f>
-        <v>1.0001656810075503</v>
+        <v>2698.3985165205663</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
@@ -16235,14 +16219,14 @@
         <v>8.3333299999999999E-8</v>
       </c>
       <c r="V5" s="4">
-        <v>0.1251899048748</v>
+        <v>2.26E-6</v>
       </c>
       <c r="W5" s="4">
         <v>4.0177499999999998E-6</v>
       </c>
       <c r="X5" s="4">
         <f t="shared" ref="X5:X11" si="9">W5/V5</f>
-        <v>3.2093242694113984E-5</v>
+        <v>1.7777654867256636</v>
       </c>
       <c r="Y5" s="4">
         <v>8.3333299999999999E-8</v>
@@ -16262,11 +16246,11 @@
       </c>
       <c r="AD5" s="4">
         <f t="shared" ref="AD5:AD11" si="11">AA5/V5</f>
-        <v>6.2741041141960912</v>
+        <v>347546.23771274334</v>
       </c>
       <c r="AE5" s="4">
         <f t="shared" ref="AE5:AE11" si="12">AC5/X5</f>
-        <v>32.167655856384414</v>
+        <v>5.8070898215102521E-4</v>
       </c>
       <c r="AF5" s="13">
         <v>8.3333299999999999E-8</v>
@@ -16275,14 +16259,14 @@
         <v>8.3333299999999999E-8</v>
       </c>
       <c r="AH5" s="4">
-        <v>1.0044157500000001E-3</v>
+        <v>4.4560000000000002E-6</v>
       </c>
       <c r="AI5" s="4">
         <v>1.0180002499999999E-3</v>
       </c>
       <c r="AJ5" s="4">
         <f t="shared" si="3"/>
-        <v>1.0135247779617154</v>
+        <v>228.45607046678631</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
@@ -16358,14 +16342,14 @@
         <v>8.3330000000000001E-10</v>
       </c>
       <c r="V6" s="4">
-        <v>0.1250411311563</v>
+        <v>2.2354999999999999E-5</v>
       </c>
       <c r="W6" s="4">
         <v>3.9484499999999998E-5</v>
       </c>
       <c r="X6" s="4">
         <f t="shared" si="9"/>
-        <v>3.1577209542870191E-4</v>
+        <v>1.7662491612614628</v>
       </c>
       <c r="Y6" s="4">
         <v>8.3330000000000001E-10</v>
@@ -16385,11 +16369,11 @@
       </c>
       <c r="AD6" s="4">
         <f t="shared" si="11"/>
-        <v>6.2856000728541135</v>
+        <v>35158.06500137777</v>
       </c>
       <c r="AE6" s="4">
         <f t="shared" si="12"/>
-        <v>37.752267284014025</v>
+        <v>6.7493945978399951E-3</v>
       </c>
       <c r="AF6" s="13">
         <v>8.3330000000000001E-10</v>
@@ -16398,14 +16382,14 @@
         <v>8.3330000000000001E-10</v>
       </c>
       <c r="AH6" s="4">
-        <v>1.144195E-4</v>
+        <v>1.363475E-5</v>
       </c>
       <c r="AI6" s="4">
         <v>2.5300125000000002E-4</v>
       </c>
       <c r="AJ6" s="4">
         <f t="shared" si="3"/>
-        <v>2.2111724837112559</v>
+        <v>18.555620748455233</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
@@ -16481,14 +16465,14 @@
         <v>8.2999999999999998E-12</v>
       </c>
       <c r="V7" s="4">
-        <v>0.1252233435141</v>
+        <v>2.2270375E-4</v>
       </c>
       <c r="W7" s="4">
         <v>3.9374925000000002E-4</v>
       </c>
       <c r="X7" s="4">
         <f t="shared" si="9"/>
-        <v>3.1443757924868401E-3</v>
+        <v>1.7680405022367158</v>
       </c>
       <c r="Y7" s="4">
         <v>8.3999999999999998E-12</v>
@@ -16508,11 +16492,11 @@
       </c>
       <c r="AD7" s="4">
         <f t="shared" si="11"/>
-        <v>6.3284384437496595</v>
+        <v>3558.3963949843683</v>
       </c>
       <c r="AE7" s="4">
         <f t="shared" si="12"/>
-        <v>32.502325128112012</v>
+        <v>5.780383662200124E-2</v>
       </c>
       <c r="AF7" s="13">
         <v>8.2999999999999998E-12</v>
@@ -16521,14 +16505,14 @@
         <v>8.2999999999999998E-12</v>
       </c>
       <c r="AH7" s="4">
-        <v>1.2430349999999999E-4</v>
+        <v>1.153355E-4</v>
       </c>
       <c r="AI7" s="4">
         <v>1.5243875E-3</v>
       </c>
       <c r="AJ7" s="4">
         <f t="shared" si="3"/>
-        <v>12.263431842224879</v>
+        <v>13.216984363010521</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
@@ -16604,14 +16588,14 @@
         <v>1E-13</v>
       </c>
       <c r="V8" s="4">
-        <v>0.12722766850010001</v>
+        <v>2.2259315000000002E-3</v>
       </c>
       <c r="W8" s="4">
         <v>3.9488709999999996E-3</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" si="9"/>
-        <v>3.1037831994829769E-2</v>
+        <v>1.7740307821691725</v>
       </c>
       <c r="Y8" s="4">
         <v>0</v>
@@ -16631,11 +16615,11 @@
       </c>
       <c r="AD8" s="4">
         <f t="shared" si="11"/>
-        <v>6.6139396627922853</v>
+        <v>378.0332516510054</v>
       </c>
       <c r="AE8" s="4">
         <f t="shared" si="12"/>
-        <v>31.077653870956667</v>
+        <v>0.54372393609810599</v>
       </c>
       <c r="AF8" s="13">
         <v>1E-13</v>
@@ -16644,14 +16628,14 @@
         <v>1E-13</v>
       </c>
       <c r="AH8" s="4">
-        <v>1.131108E-3</v>
+        <v>1.1253382499999999E-3</v>
       </c>
       <c r="AI8" s="4">
         <v>1.50827485E-2</v>
       </c>
       <c r="AJ8" s="4">
         <f t="shared" si="3"/>
-        <v>13.334490163627169</v>
+        <v>13.402857762988152</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.3">
@@ -16727,14 +16711,14 @@
         <v>0</v>
       </c>
       <c r="V9" s="4">
-        <v>0.14086739300000001</v>
+        <v>1.5621757999999999E-2</v>
       </c>
       <c r="W9" s="4">
         <v>2.4076813249999999E-2</v>
       </c>
       <c r="X9" s="4">
         <f t="shared" si="9"/>
-        <v>0.17091828518470556</v>
+        <v>1.5412358359411278</v>
       </c>
       <c r="Y9" s="4">
         <v>1E-13</v>
@@ -16754,11 +16738,11 @@
       </c>
       <c r="AD9" s="4">
         <f t="shared" si="11"/>
-        <v>9.5568705928092239</v>
+        <v>86.177973416781896</v>
       </c>
       <c r="AE9" s="4">
         <f t="shared" si="12"/>
-        <v>35.104527141961846</v>
+        <v>3.8929834366719591</v>
       </c>
       <c r="AF9" s="13">
         <v>0</v>
@@ -16767,14 +16751,14 @@
         <v>1E-13</v>
       </c>
       <c r="AH9" s="4">
-        <v>1.12947415E-2</v>
+        <v>1.06350695E-2</v>
       </c>
       <c r="AI9" s="4">
         <v>0.15197584524999999</v>
       </c>
       <c r="AJ9" s="4">
         <f t="shared" si="3"/>
-        <v>13.455451393022141</v>
+        <v>14.290066016963969</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.3">
@@ -16850,14 +16834,14 @@
         <v>0</v>
       </c>
       <c r="V10" s="4">
-        <v>0.25487476662500003</v>
+        <v>0.12996826175000001</v>
       </c>
       <c r="W10" s="4">
         <v>0.2299231605</v>
       </c>
       <c r="X10" s="4">
         <f t="shared" si="9"/>
-        <v>0.90210248564263884</v>
+        <v>1.7690715979741876</v>
       </c>
       <c r="Y10" s="4">
         <v>5.9999999999999997E-13</v>
@@ -16877,11 +16861,11 @@
       </c>
       <c r="AD10" s="4">
         <f t="shared" si="11"/>
-        <v>25.085090333028173</v>
+        <v>49.193214237918355</v>
       </c>
       <c r="AE10" s="4">
         <f t="shared" si="12"/>
-        <v>13.92835744506865</v>
+        <v>7.1024857820926464</v>
       </c>
       <c r="AF10" s="13">
         <v>0</v>
@@ -16890,14 +16874,14 @@
         <v>1E-13</v>
       </c>
       <c r="AH10" s="4">
-        <v>5.6541675999999999E-2</v>
+        <v>5.6411853249999998E-2</v>
       </c>
       <c r="AI10" s="4">
         <v>1.5126712772499999</v>
       </c>
       <c r="AJ10" s="4">
         <f t="shared" si="3"/>
-        <v>26.753209035579349</v>
+        <v>26.814777216169546</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
@@ -16973,14 +16957,14 @@
         <v>0</v>
       </c>
       <c r="V11" s="4">
-        <v>1.4227878419375</v>
+        <v>1.3005261925</v>
       </c>
       <c r="W11" s="4">
         <v>2.299802997</v>
       </c>
       <c r="X11" s="4">
         <f t="shared" si="9"/>
-        <v>1.6164061353435613</v>
+        <v>1.7683634595463944</v>
       </c>
       <c r="Y11" s="4">
         <v>2.0000000000000001E-13</v>
@@ -17000,11 +16984,11 @@
       </c>
       <c r="AD11" s="4">
         <f t="shared" si="11"/>
-        <v>39.970655371889009</v>
+        <v>43.728271545286468</v>
       </c>
       <c r="AE11" s="4">
         <f t="shared" si="12"/>
-        <v>8.7260153582315869</v>
+        <v>7.97617971916572</v>
       </c>
       <c r="AF11" s="13">
         <v>0</v>
@@ -17013,14 +16997,14 @@
         <v>0</v>
       </c>
       <c r="AH11" s="4">
-        <v>0.56208813224999998</v>
+        <v>0.56460486200000004</v>
       </c>
       <c r="AI11" s="4">
         <v>15.064032785249999</v>
       </c>
       <c r="AJ11" s="4">
         <f t="shared" si="3"/>
-        <v>26.800126031748288</v>
+        <v>26.680664300141995</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
@@ -17042,15 +17026,15 @@
       </c>
       <c r="AD12" s="4">
         <f>AVERAGE(AD4:AD11)</f>
-        <v>13.288048939147231</v>
+        <v>382852.53082195792</v>
       </c>
       <c r="AE12" s="4">
         <f>AVERAGE(AE4:AE11)</f>
-        <v>27.355392183753274</v>
+        <v>2.4475713272337276</v>
       </c>
       <c r="AJ12" s="4">
         <f>AVERAGE(AJ4:AJ11)</f>
-        <v>12.103946426110294</v>
+        <v>379.97694467438527</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
@@ -17072,15 +17056,15 @@
       </c>
       <c r="AD13" s="4">
         <f>MAX(AD4:AD11)-MIN(AD4:AD11)</f>
-        <v>33.780962450029719</v>
+        <v>2675956.6864841618</v>
       </c>
       <c r="AE13" s="4">
         <f>MAX(AE4:AE11)-MIN(AE4:AE11)</f>
-        <v>29.026251925782439</v>
+        <v>7.9761159155263233</v>
       </c>
       <c r="AJ13" s="4">
         <f>MAX(AJ4:AJ11)-MIN(AJ4:AJ11)</f>
-        <v>25.799960350740736</v>
+        <v>2685.1815321575559</v>
       </c>
     </row>
   </sheetData>
@@ -17116,7 +17100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1CE195-C062-47CA-8580-D3479DE98BDB}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H28" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
@@ -17344,11 +17328,11 @@
         <v>0.169187</v>
       </c>
       <c r="G4" s="4">
-        <f>F4/E4</f>
+        <f t="shared" ref="G4:G11" si="0">F4/E4</f>
         <v>17.744977114352718</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H11" si="0">E4/B4</f>
+        <f t="shared" ref="H4:H11" si="1">E4/B4</f>
         <v>4.7300725806051522</v>
       </c>
       <c r="I4" s="4">
@@ -17362,7 +17346,7 @@
         <v>5.95985E-3</v>
       </c>
       <c r="L4" s="4">
-        <f>K4/J4</f>
+        <f t="shared" ref="L4:L11" si="2">K4/J4</f>
         <v>3.2176619534291095</v>
       </c>
       <c r="M4" s="4">
@@ -17376,7 +17360,7 @@
         <v>28.508556060802036</v>
       </c>
       <c r="P4" s="4">
-        <f t="shared" ref="P4:P11" si="1">M4/J4</f>
+        <f t="shared" ref="P4:P11" si="3">M4/J4</f>
         <v>3.2140122986886079</v>
       </c>
       <c r="Q4" s="4">
@@ -17404,11 +17388,11 @@
         <v>28.571812879459145</v>
       </c>
       <c r="X4" s="4">
-        <f>U4/R4</f>
+        <f t="shared" ref="X4:X11" si="4">U4/R4</f>
         <v>6.5894924605856477</v>
       </c>
       <c r="Y4" s="4">
-        <f>W4/T4</f>
+        <f t="shared" ref="Y4:Y11" si="5">W4/T4</f>
         <v>7.4244581317446317</v>
       </c>
       <c r="Z4" s="4">
@@ -17418,7 +17402,7 @@
         <v>2.6198200000000001E-3</v>
       </c>
       <c r="AB4" s="4">
-        <f t="shared" ref="AB4:AB11" si="2">AA4/Z4</f>
+        <f t="shared" ref="AB4:AB11" si="6">AA4/Z4</f>
         <v>5.4071089793070994</v>
       </c>
     </row>
@@ -17433,7 +17417,7 @@
         <v>2.8602499999999999E-2</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D13" si="3">C5/B5</f>
+        <f t="shared" ref="D5:D13" si="7">C5/B5</f>
         <v>2.7092114610466496</v>
       </c>
       <c r="E5" s="4">
@@ -17443,15 +17427,15 @@
         <v>1.3817900000000001</v>
       </c>
       <c r="G5" s="4">
-        <f>F5/E5</f>
+        <f t="shared" si="0"/>
         <v>14.13445526000303</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2598058252427187</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I11" si="4">G5/D5</f>
+        <f t="shared" ref="I5:I11" si="8">G5/D5</f>
         <v>5.2171842114319364</v>
       </c>
       <c r="J5" s="4">
@@ -17461,7 +17445,7 @@
         <v>1.7787399999999998E-2</v>
       </c>
       <c r="L5" s="4">
-        <f>K5/J5</f>
+        <f t="shared" si="2"/>
         <v>1.6993302953006026</v>
       </c>
       <c r="M5" s="4">
@@ -17471,15 +17455,15 @@
         <v>1.3921399999999999</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" ref="O5:O13" si="5">N5/M5</f>
+        <f t="shared" ref="O5:O13" si="9">N5/M5</f>
         <v>24.034694874667874</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.533623761619519</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" ref="Q5:Q11" si="6">O5/L5</f>
+        <f t="shared" ref="Q5:Q11" si="10">O5/L5</f>
         <v>14.143627605024403</v>
       </c>
       <c r="R5" s="4">
@@ -17489,7 +17473,7 @@
         <v>2.7380700000000001E-2</v>
       </c>
       <c r="T5" s="4">
-        <f t="shared" ref="T5:T13" si="7">S5/R5</f>
+        <f t="shared" ref="T5:T13" si="11">S5/R5</f>
         <v>3.5322916478532007</v>
       </c>
       <c r="U5" s="4">
@@ -17499,15 +17483,15 @@
         <v>1.3868400000000001</v>
       </c>
       <c r="W5" s="4">
-        <f t="shared" ref="W5:W13" si="8">V5/U5</f>
+        <f t="shared" ref="W5:W13" si="12">V5/U5</f>
         <v>23.5629928283441</v>
       </c>
       <c r="X5" s="4">
-        <f>U5/R5</f>
+        <f t="shared" si="4"/>
         <v>7.5929041196975042</v>
       </c>
       <c r="Y5" s="4">
-        <f>W5/T5</f>
+        <f t="shared" si="5"/>
         <v>6.6707381998496178</v>
       </c>
       <c r="Z5" s="4">
@@ -17517,7 +17501,7 @@
         <v>2.5305500000000002E-2</v>
       </c>
       <c r="AB5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>6.5207420176923661</v>
       </c>
     </row>
@@ -17532,7 +17516,7 @@
         <v>9.6381499999999995E-2</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.2949226409040673</v>
       </c>
       <c r="E6" s="4">
@@ -17542,15 +17526,15 @@
         <v>4.8069600000000001</v>
       </c>
       <c r="G6" s="4">
-        <f>F6/E6</f>
+        <f t="shared" si="0"/>
         <v>12.886981279272083</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.621911874799473</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3.000515342590528</v>
       </c>
       <c r="J6" s="4">
@@ -17560,7 +17544,7 @@
         <v>5.95148E-2</v>
       </c>
       <c r="L6" s="4">
-        <f>K6/J6</f>
+        <f t="shared" si="2"/>
         <v>2.819203713791715</v>
       </c>
       <c r="M6" s="4">
@@ -17570,15 +17554,15 @@
         <v>4.7998000000000003</v>
       </c>
       <c r="O6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>20.995030968961053</v>
       </c>
       <c r="P6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.829492432675684</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>7.4471493018585688</v>
       </c>
       <c r="R6" s="4">
@@ -17588,7 +17572,7 @@
         <v>9.1636599999999999E-2</v>
       </c>
       <c r="T6" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>7.0539612648951566</v>
       </c>
       <c r="U6" s="4">
@@ -17598,15 +17582,15 @@
         <v>4.8210199999999999</v>
       </c>
       <c r="W6" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>21.109364532386387</v>
       </c>
       <c r="X6" s="4">
-        <f>U6/R6</f>
+        <f t="shared" si="4"/>
         <v>17.580364565692644</v>
       </c>
       <c r="Y6" s="4">
-        <f>W6/T6</f>
+        <f t="shared" si="5"/>
         <v>2.9925546426572467</v>
       </c>
       <c r="Z6" s="4">
@@ -17616,7 +17600,7 @@
         <v>9.5278699999999994E-2</v>
       </c>
       <c r="AB6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>7.1430274314588376</v>
       </c>
     </row>
@@ -17631,7 +17615,7 @@
         <v>0.23596500000000001</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.3274891338236108</v>
       </c>
       <c r="E7" s="4">
@@ -17641,15 +17625,15 @@
         <v>12.648899999999999</v>
       </c>
       <c r="G7" s="4">
-        <f>F7/E7</f>
+        <f t="shared" si="0"/>
         <v>7.7402595813165096</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.969923157334897</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.7886260004256787</v>
       </c>
       <c r="J7" s="4">
@@ -17659,7 +17643,7 @@
         <v>0.147178</v>
       </c>
       <c r="L7" s="4">
-        <f>K7/J7</f>
+        <f t="shared" si="2"/>
         <v>2.8860129027197678</v>
       </c>
       <c r="M7" s="4">
@@ -17669,15 +17653,15 @@
         <v>12.6776</v>
       </c>
       <c r="O7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9.5677111634365755</v>
       </c>
       <c r="P7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25.982704864992058</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.3152004117583811</v>
       </c>
       <c r="R7" s="4">
@@ -17687,7 +17671,7 @@
         <v>0.22106300000000001</v>
       </c>
       <c r="T7" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.8886535874588786</v>
       </c>
       <c r="U7" s="4">
@@ -17697,15 +17681,15 @@
         <v>12.551399999999999</v>
       </c>
       <c r="W7" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9.9273132805517541</v>
       </c>
       <c r="X7" s="4">
-        <f>U7/R7</f>
+        <f t="shared" si="4"/>
         <v>33.679093245961027</v>
       </c>
       <c r="Y7" s="4">
-        <f>W7/T7</f>
+        <f t="shared" si="5"/>
         <v>1.6858375404683419</v>
       </c>
       <c r="Z7" s="4">
@@ -17715,7 +17699,7 @@
         <v>0.44961200000000001</v>
       </c>
       <c r="AB7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>22.703319564931984</v>
       </c>
     </row>
@@ -17730,7 +17714,7 @@
         <v>0.60554699999999995</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>5.7356501477608539</v>
       </c>
       <c r="E8" s="4">
@@ -17740,15 +17724,15 @@
         <v>26.038900000000002</v>
       </c>
       <c r="G8" s="4">
-        <f>F8/E8</f>
+        <f t="shared" si="0"/>
         <v>8.5787755290303664</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.749621126013487</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.4956936542545998</v>
       </c>
       <c r="J8" s="4">
@@ -17758,7 +17742,7 @@
         <v>0.43921500000000002</v>
       </c>
       <c r="L8" s="4">
-        <f>K8/J8</f>
+        <f t="shared" si="2"/>
         <v>4.3691681753974096</v>
       </c>
       <c r="M8" s="4">
@@ -17768,15 +17752,15 @@
         <v>26.2273</v>
       </c>
       <c r="O8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10.259907913421403</v>
       </c>
       <c r="P8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25.429142709348827</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.3482520016497612</v>
       </c>
       <c r="R8" s="4">
@@ -17786,7 +17770,7 @@
         <v>0.62780100000000005</v>
       </c>
       <c r="T8" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8.2798118251561856</v>
       </c>
       <c r="U8" s="4">
@@ -17796,15 +17780,15 @@
         <v>26.135300000000001</v>
       </c>
       <c r="W8" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>11.491883002673422</v>
       </c>
       <c r="X8" s="4">
-        <f>U8/R8</f>
+        <f t="shared" si="4"/>
         <v>29.994025567406236</v>
       </c>
       <c r="Y8" s="4">
-        <f>W8/T8</f>
+        <f t="shared" si="5"/>
         <v>1.3879401181266153</v>
       </c>
       <c r="Z8" s="4">
@@ -17814,7 +17798,7 @@
         <v>1.0150300000000001</v>
       </c>
       <c r="AB8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>25.852535383816029</v>
       </c>
     </row>
@@ -17829,7 +17813,7 @@
         <v>0.873672</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.704546923126629</v>
       </c>
       <c r="E9" s="4">
@@ -17839,15 +17823,15 @@
         <v>46.448900000000002</v>
       </c>
       <c r="G9" s="4">
-        <f>F9/E9</f>
+        <f t="shared" si="0"/>
         <v>6.0998187739664864</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41.004157063777541</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.2965794312691357</v>
       </c>
       <c r="J9" s="4">
@@ -17857,7 +17841,7 @@
         <v>0.57806599999999997</v>
       </c>
       <c r="L9" s="4">
-        <f>K9/J9</f>
+        <f t="shared" si="2"/>
         <v>3.2919851023360174</v>
       </c>
       <c r="M9" s="4">
@@ -17867,15 +17851,15 @@
         <v>46.599499999999999</v>
       </c>
       <c r="O9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.2581047109654619</v>
       </c>
       <c r="P9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>36.562717115229106</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.2047805458825001</v>
       </c>
       <c r="R9" s="4">
@@ -17885,7 +17869,7 @@
         <v>0.854904</v>
       </c>
       <c r="T9" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.5455714810731349</v>
       </c>
       <c r="U9" s="4">
@@ -17895,15 +17879,15 @@
         <v>46.6614</v>
       </c>
       <c r="W9" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7.1833405688000518</v>
       </c>
       <c r="X9" s="4">
-        <f>U9/R9</f>
+        <f t="shared" si="4"/>
         <v>49.734932010290336</v>
       </c>
       <c r="Y9" s="4">
-        <f>W9/T9</f>
+        <f t="shared" si="5"/>
         <v>1.097435203262398</v>
       </c>
       <c r="Z9" s="4">
@@ -17913,7 +17897,7 @@
         <v>2.0329899999999999</v>
       </c>
       <c r="AB9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>29.778847393276067</v>
       </c>
     </row>
@@ -17928,7 +17912,7 @@
         <v>1.4330700000000001</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.6406655289549787</v>
       </c>
       <c r="E10" s="4">
@@ -17938,15 +17922,15 @@
         <v>73.738100000000003</v>
       </c>
       <c r="G10" s="4">
-        <f>F10/E10</f>
+        <f t="shared" si="0"/>
         <v>5.3204011688733361</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44.88078314286917</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.1464737408195469</v>
       </c>
       <c r="J10" s="4">
@@ -17956,7 +17940,7 @@
         <v>1.0108600000000001</v>
       </c>
       <c r="L10" s="4">
-        <f>K10/J10</f>
+        <f t="shared" si="2"/>
         <v>3.4142947373398589</v>
       </c>
       <c r="M10" s="4">
@@ -17966,15 +17950,15 @@
         <v>73.997299999999996</v>
       </c>
       <c r="O10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.2127264789347301</v>
       </c>
       <c r="P10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40.229407532754408</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.8196221934182466</v>
       </c>
       <c r="R10" s="4">
@@ -17984,7 +17968,7 @@
         <v>1.21163</v>
       </c>
       <c r="T10" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.3392941342370017</v>
       </c>
       <c r="U10" s="4">
@@ -17994,15 +17978,15 @@
         <v>74.131500000000003</v>
       </c>
       <c r="W10" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6.1995818523938953</v>
       </c>
       <c r="X10" s="4">
-        <f>U10/R10</f>
+        <f t="shared" si="4"/>
         <v>52.693156830170054</v>
       </c>
       <c r="Y10" s="4">
-        <f>W10/T10</f>
+        <f t="shared" si="5"/>
         <v>1.1611238670371231</v>
       </c>
       <c r="Z10" s="4">
@@ -18012,7 +17996,7 @@
         <v>3.7886600000000001</v>
       </c>
       <c r="AB10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>34.722988516281589</v>
       </c>
     </row>
@@ -18027,7 +18011,7 @@
         <v>2.6095600000000001</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.5891087890096056</v>
       </c>
       <c r="E11" s="4">
@@ -18037,15 +18021,15 @@
         <v>110.40300000000001</v>
       </c>
       <c r="G11" s="4">
-        <f>F11/E11</f>
+        <f t="shared" si="0"/>
         <v>5.0471788682557541</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.467436453867279</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.0998167836733734</v>
       </c>
       <c r="J11" s="4">
@@ -18055,7 +18039,7 @@
         <v>1.9441900000000001</v>
       </c>
       <c r="L11" s="4">
-        <f>K11/J11</f>
+        <f t="shared" si="2"/>
         <v>3.5065895436648575</v>
       </c>
       <c r="M11" s="4">
@@ -18065,15 +18049,15 @@
         <v>111.633</v>
       </c>
       <c r="O11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5.8736898598307858</v>
       </c>
       <c r="P11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34.278973881707458</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.67504345367208</v>
       </c>
       <c r="R11" s="4">
@@ -18083,7 +18067,7 @@
         <v>2.2316500000000001</v>
       </c>
       <c r="T11" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.1076622371956555</v>
       </c>
       <c r="U11" s="4">
@@ -18093,15 +18077,15 @@
         <v>111.40600000000001</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5.9024922646547706</v>
       </c>
       <c r="X11" s="4">
-        <f>U11/R11</f>
+        <f t="shared" si="4"/>
         <v>43.198557179542348</v>
       </c>
       <c r="Y11" s="4">
-        <f>W11/T11</f>
+        <f t="shared" si="5"/>
         <v>1.1556152287578658</v>
       </c>
       <c r="Z11" s="4">
@@ -18111,7 +18095,7 @@
         <v>5.8071099999999998</v>
       </c>
       <c r="AB11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>25.006933080699334</v>
       </c>
     </row>
@@ -18126,7 +18110,7 @@
         <v>3.1626300000000001</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.8404595975970945</v>
       </c>
       <c r="E12" s="4">
@@ -18136,7 +18120,7 @@
         <v>157.53899999999999</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" ref="G12:G13" si="9">F12/E12</f>
+        <f t="shared" ref="G12:G13" si="13">F12/E12</f>
         <v>4.7641930245287636</v>
       </c>
       <c r="H12" s="4">
@@ -18154,7 +18138,7 @@
         <v>2.22695</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12:L13" si="10">K12/J12</f>
+        <f t="shared" ref="L12:L13" si="14">K12/J12</f>
         <v>2.8045251216538882</v>
       </c>
       <c r="M12" s="4">
@@ -18164,7 +18148,7 @@
         <v>158.82599999999999</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5.4378871035665739</v>
       </c>
       <c r="P12" s="4">
@@ -18182,7 +18166,7 @@
         <v>2.4108200000000002</v>
       </c>
       <c r="T12" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.8296831339980848</v>
       </c>
       <c r="U12" s="4">
@@ -18192,7 +18176,7 @@
         <v>158.74799999999999</v>
       </c>
       <c r="W12" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5.4872952392145207</v>
       </c>
       <c r="X12" s="4">
@@ -18225,7 +18209,7 @@
         <v>4.2176400000000003</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3.3867105632954595</v>
       </c>
       <c r="E13" s="4">
@@ -18235,7 +18219,7 @@
         <v>220.959</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4.7581711450585509</v>
       </c>
       <c r="H13" s="4">
@@ -18253,7 +18237,7 @@
         <v>3.0288499999999998</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.5547842369850535</v>
       </c>
       <c r="M13" s="4">
@@ -18263,7 +18247,7 @@
         <v>222.268</v>
       </c>
       <c r="O13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5.4418764077955144</v>
       </c>
       <c r="P13" s="4">
@@ -18281,7 +18265,7 @@
         <v>3.31413</v>
       </c>
       <c r="T13" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.4028141421733213</v>
       </c>
       <c r="U13" s="4">
@@ -18291,7 +18275,7 @@
         <v>222.172</v>
       </c>
       <c r="W13" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5.4060130617170996</v>
       </c>
       <c r="X13" s="4">

</xml_diff>